<commit_message>
formatting cell variable solved
</commit_message>
<xml_diff>
--- a/User Data/Feburary/sample.xlsx
+++ b/User Data/Feburary/sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bill Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="template" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="temp" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="temp1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Bill Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="template" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="temp" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="temp1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="12" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -2442,6 +2443,551 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A2:H45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.140625" customWidth="1" style="64" min="1" max="3"/>
+    <col width="14.85546875" customWidth="1" style="64" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="64" min="5" max="7"/>
+    <col width="13.85546875" customWidth="1" style="64" min="8" max="8"/>
+    <col width="9.140625" customWidth="1" style="64" min="9" max="58"/>
+    <col width="9.140625" customWidth="1" style="64" min="59" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="120.75" customHeight="1" s="64" thickBot="1"/>
+    <row r="2" ht="15.75" customHeight="1" s="64">
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="33" t="n"/>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D2" s="72" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="E2" s="70" t="n"/>
+      <c r="F2" s="71" t="n"/>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="16.5" customHeight="1" s="64" thickBot="1">
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="33" t="n"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>STRN</t>
+        </is>
+      </c>
+      <c r="D3" s="72" t="inlineStr">
+        <is>
+          <t>8187702-6</t>
+        </is>
+      </c>
+      <c r="E3" s="70" t="n"/>
+      <c r="F3" s="71" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="16.5" customHeight="1" s="64" thickBot="1">
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="33" t="n"/>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>NTN</t>
+        </is>
+      </c>
+      <c r="D4" s="72" t="inlineStr">
+        <is>
+          <t>35101-2935417-3</t>
+        </is>
+      </c>
+      <c r="E4" s="70" t="n"/>
+      <c r="F4" s="71" t="n"/>
+      <c r="G4" s="4" t="n"/>
+      <c r="H4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="16.5" customHeight="1" s="64" thickBot="1">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="33" t="n"/>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>AC/NO</t>
+        </is>
+      </c>
+      <c r="D5" s="73" t="inlineStr">
+        <is>
+          <t>0018 0981 0217 5901</t>
+        </is>
+      </c>
+      <c r="E5" s="70" t="n"/>
+      <c r="F5" s="71" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="21" customHeight="1" s="64">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="33" t="n"/>
+      <c r="C6" s="33" t="n"/>
+      <c r="D6" s="33" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" s="64">
+      <c r="A7" s="30" t="inlineStr">
+        <is>
+          <t>10/Feb/2021</t>
+        </is>
+      </c>
+      <c r="B7" s="30" t="n"/>
+      <c r="C7" s="30" t="n"/>
+      <c r="D7" s="33" t="n"/>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="63" t="inlineStr">
+        <is>
+          <t>Complaint No.</t>
+        </is>
+      </c>
+      <c r="G7" s="63" t="n"/>
+      <c r="H7" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" s="64">
+      <c r="A8" s="33" t="inlineStr">
+        <is>
+          <t>Bank Al Habib Limited</t>
+        </is>
+      </c>
+      <c r="B8" s="33" t="n"/>
+      <c r="C8" s="33" t="n"/>
+      <c r="D8" s="33" t="n"/>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n"/>
+      <c r="G8" s="4" t="n"/>
+      <c r="H8" s="5" t="n"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="64">
+      <c r="A9" s="33" t="inlineStr">
+        <is>
+          <t>sample  Branch,sample Zone</t>
+        </is>
+      </c>
+      <c r="B9" s="33" t="n"/>
+      <c r="C9" s="33" t="n"/>
+      <c r="D9" s="32" t="n"/>
+      <c r="E9" s="4" t="n"/>
+      <c r="F9" s="4" t="n"/>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="64">
+      <c r="A10" s="74" t="n"/>
+      <c r="D10" s="33" t="n"/>
+      <c r="E10" s="4" t="n"/>
+      <c r="F10" s="4" t="n"/>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" s="64">
+      <c r="A11" s="32" t="n"/>
+      <c r="B11" s="32" t="n"/>
+      <c r="C11" s="32" t="n"/>
+      <c r="D11" s="33" t="n"/>
+      <c r="E11" s="4" t="n"/>
+      <c r="F11" s="4" t="n"/>
+      <c r="G11" s="4" t="n"/>
+      <c r="H11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="63" t="inlineStr">
+        <is>
+          <t>Subject:      Bill for subject_line:</t>
+        </is>
+      </c>
+      <c r="B12" s="63" t="n"/>
+      <c r="C12" s="63" t="n"/>
+      <c r="D12" s="63" t="n"/>
+      <c r="E12" s="63" t="n"/>
+      <c r="F12" s="63" t="n"/>
+      <c r="G12" s="63" t="n"/>
+      <c r="H12" s="63" t="n"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="64">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="33" t="n"/>
+      <c r="C13" s="33" t="n"/>
+      <c r="D13" s="33" t="n"/>
+      <c r="E13" s="4" t="n"/>
+      <c r="F13" s="4" t="n"/>
+      <c r="G13" s="4" t="n"/>
+      <c r="H13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="69" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
+      <c r="B14" s="70" t="n"/>
+      <c r="C14" s="70" t="n"/>
+      <c r="D14" s="70" t="n"/>
+      <c r="E14" s="70" t="n"/>
+      <c r="F14" s="70" t="n"/>
+      <c r="G14" s="70" t="n"/>
+      <c r="H14" s="71" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="69" t="inlineStr">
+        <is>
+          <t>Sr No</t>
+        </is>
+      </c>
+      <c r="B15" s="69" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C15" s="70" t="n"/>
+      <c r="D15" s="71" t="n"/>
+      <c r="E15" s="69" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="F15" s="69" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="G15" s="69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate </t>
+        </is>
+      </c>
+      <c r="H15" s="6" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="31.5" customHeight="1" s="64">
+      <c r="A16" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="75" t="inlineStr">
+        <is>
+          <t>PCB kit Repair with aeroflex installation outdoor</t>
+        </is>
+      </c>
+      <c r="C16" s="70" t="n"/>
+      <c r="D16" s="71" t="n"/>
+      <c r="E16" s="40" t="inlineStr">
+        <is>
+          <t>45rft</t>
+        </is>
+      </c>
+      <c r="F16" s="73" t="n"/>
+      <c r="G16" s="40" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H16" s="41" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" s="64">
+      <c r="A17" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="76" t="inlineStr">
+        <is>
+          <t>Gas charging</t>
+        </is>
+      </c>
+      <c r="C17" s="70" t="n"/>
+      <c r="D17" s="71" t="n"/>
+      <c r="E17" s="42" t="inlineStr">
+        <is>
+          <t>45rft</t>
+        </is>
+      </c>
+      <c r="F17" s="43" t="n"/>
+      <c r="G17" s="42" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H17" s="44" t="n">
+        <v>23445.78</v>
+      </c>
+    </row>
+    <row r="18" ht="31.5" customHeight="1" s="64">
+      <c r="A18" s="42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="76" t="inlineStr">
+        <is>
+          <t>Coil brazing on new Heir AC outdoor installation</t>
+        </is>
+      </c>
+      <c r="C18" s="70" t="n"/>
+      <c r="D18" s="71" t="n"/>
+      <c r="E18" s="42" t="inlineStr">
+        <is>
+          <t>45rft</t>
+        </is>
+      </c>
+      <c r="F18" s="43" t="n"/>
+      <c r="G18" s="42" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H18" s="44" t="n">
+        <v>234.89</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="64">
+      <c r="A19" s="40" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="75" t="inlineStr">
+        <is>
+          <t>Gas charging</t>
+        </is>
+      </c>
+      <c r="C19" s="70" t="n"/>
+      <c r="D19" s="71" t="n"/>
+      <c r="E19" s="40" t="inlineStr">
+        <is>
+          <t>45rft</t>
+        </is>
+      </c>
+      <c r="F19" s="73" t="n"/>
+      <c r="G19" s="40" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H19" s="41" t="n">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" s="64">
+      <c r="A20" s="45" t="n"/>
+      <c r="B20" s="77" t="n"/>
+      <c r="C20" s="70" t="n"/>
+      <c r="D20" s="70" t="n"/>
+      <c r="E20" s="46" t="n"/>
+      <c r="F20" s="22" t="n"/>
+      <c r="G20" s="46" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="H20" s="47">
+        <f>SUM(H16:H19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" s="64">
+      <c r="A21" s="21" t="n"/>
+      <c r="B21" s="22" t="n"/>
+      <c r="C21" s="22" t="n"/>
+      <c r="D21" s="22" t="n"/>
+      <c r="E21" s="22" t="n"/>
+      <c r="F21" s="22" t="n"/>
+      <c r="G21" s="22" t="inlineStr">
+        <is>
+          <t>Tax (16%)</t>
+        </is>
+      </c>
+      <c r="H21" s="31">
+        <f>H20*0.16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="64">
+      <c r="A22" s="73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B22" s="26" t="inlineStr">
+        <is>
+          <t>extra Charges</t>
+        </is>
+      </c>
+      <c r="C22" s="27" t="n"/>
+      <c r="D22" s="28" t="n"/>
+      <c r="E22" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>780</v>
+      </c>
+      <c r="H22" s="8" t="n">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B23" s="26" t="inlineStr">
+        <is>
+          <t>Out of City Charges</t>
+        </is>
+      </c>
+      <c r="C23" s="27" t="n"/>
+      <c r="D23" s="28" t="n"/>
+      <c r="E23" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="21" t="n"/>
+      <c r="B24" s="22" t="n"/>
+      <c r="C24" s="22" t="n"/>
+      <c r="D24" s="22" t="n"/>
+      <c r="E24" s="22" t="n"/>
+      <c r="F24" s="22" t="n"/>
+      <c r="G24" s="22" t="inlineStr">
+        <is>
+          <t>Total Amount</t>
+        </is>
+      </c>
+      <c r="H24" s="9">
+        <f>SUM(H20:H23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" s="64">
+      <c r="A25" s="34" t="n"/>
+      <c r="B25" s="34" t="n"/>
+      <c r="C25" s="34" t="n"/>
+      <c r="D25" s="34" t="n"/>
+      <c r="E25" s="34" t="n"/>
+      <c r="F25" s="34" t="n"/>
+      <c r="G25" s="34" t="n"/>
+      <c r="H25" s="34" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="34" t="n"/>
+      <c r="B26" s="34" t="n"/>
+      <c r="C26" s="34" t="n"/>
+      <c r="D26" s="34" t="n"/>
+      <c r="E26" s="34" t="n"/>
+      <c r="F26" s="34" t="n"/>
+      <c r="G26" s="34" t="n"/>
+      <c r="H26" s="34" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="33" t="inlineStr">
+        <is>
+          <t>Truly Yours,</t>
+        </is>
+      </c>
+      <c r="B27" s="33" t="n"/>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="10" t="n"/>
+      <c r="E27" s="10" t="n"/>
+      <c r="F27" s="10" t="n"/>
+      <c r="G27" s="10" t="n"/>
+      <c r="H27" s="10" t="n"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" s="64">
+      <c r="A28" s="34" t="n"/>
+      <c r="B28" s="34" t="n"/>
+      <c r="C28" s="34" t="n"/>
+      <c r="D28" s="34" t="n"/>
+      <c r="E28" s="34" t="n"/>
+      <c r="F28" s="34" t="n"/>
+      <c r="G28" s="34" t="n"/>
+      <c r="H28" s="34" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="29" t="inlineStr">
+        <is>
+          <t>ASAD ALI</t>
+        </is>
+      </c>
+      <c r="B29" s="29" t="n"/>
+      <c r="C29" s="10" t="n"/>
+      <c r="D29" s="10" t="n"/>
+      <c r="E29" s="10" t="n"/>
+      <c r="F29" s="10" t="n"/>
+      <c r="G29" s="10" t="n"/>
+      <c r="H29" s="10" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   (Chief Executive)</t>
+        </is>
+      </c>
+      <c r="B30" s="33" t="n"/>
+      <c r="C30" s="10" t="n"/>
+      <c r="D30" s="10" t="n"/>
+      <c r="E30" s="10" t="n"/>
+      <c r="F30" s="10" t="n"/>
+      <c r="G30" s="10" t="n"/>
+      <c r="H30" s="10" t="n"/>
+    </row>
+    <row r="45">
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2469,7 +3015,7 @@
       </c>
       <c r="D2" s="72" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" s="70" t="n"/>
@@ -2544,7 +3090,7 @@
     <row r="7" ht="15.75" customHeight="1" s="64">
       <c r="A7" s="30" t="inlineStr">
         <is>
-          <t>10/Feb/2021</t>
+          <t>15/Feb/2021</t>
         </is>
       </c>
       <c r="B7" s="30" t="n"/>
@@ -2558,7 +3104,7 @@
       </c>
       <c r="G7" s="63" t="n"/>
       <c r="H7" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="64">

</xml_diff>